<commit_message>
fix voor tel nr
</commit_message>
<xml_diff>
--- a/Vul_in.xlsx
+++ b/Vul_in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobew\OneDrive\Documents\Chiro\InschrijvingScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062402EB-2190-4684-B952-5EC91AD17AC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1936070B-3D61-469B-86C2-2ABA99659473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,12 +118,6 @@
     <t>Rakker</t>
   </si>
   <si>
-    <t>Aspi</t>
-  </si>
-  <si>
-    <t>0486000001</t>
-  </si>
-  <si>
     <t>0486000002</t>
   </si>
   <si>
@@ -139,9 +133,6 @@
     <t>Plankton</t>
   </si>
   <si>
-    <t>0486000004</t>
-  </si>
-  <si>
     <t>0486000005</t>
   </si>
   <si>
@@ -155,6 +146,15 @@
   </si>
   <si>
     <t>Krabs</t>
+  </si>
+  <si>
+    <t>Aspirant</t>
+  </si>
+  <si>
+    <t>+32486000001</t>
+  </si>
+  <si>
+    <t>0032486000004</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>20</v>
@@ -651,7 +651,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>20</v>
@@ -686,16 +686,16 @@
         <v>37148</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H5" s="4">
         <v>8</v>
@@ -715,25 +715,25 @@
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5">
         <v>37149</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8">
         <v>54</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5">
         <v>37150</v>
@@ -759,7 +759,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>20</v>
@@ -774,7 +774,7 @@
         <v>9000</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.3">
@@ -1260,9 +1260,6 @@
     <row r="177" ht="12.5" x14ac:dyDescent="0.25"/>
     <row r="178" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="m05cTEYKf5DCfNJpJapBL3oi6VyZwqRxsE2O5jtrx1nrhgPo5UBLKyVzjKFAu0n2CExCY+WgGY0BzXD44f7YFQ==" saltValue="vfQOO3J9A50pTaZ/yt2/zw==" spinCount="100000" sqref="A1:XFD1" name="Range1"/>
-  </protectedRanges>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">

</xml_diff>